<commit_message>
refactoring and reading current processes from local machine with tested convention
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeniorDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CE80384-7ABF-417E-B526-3997FF950D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CEF00F-67E5-46AB-81DD-329BF32AE176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="3450" windowWidth="21600" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
+    <workbookView xWindow="28680" yWindow="1245" windowWidth="24240" windowHeight="13140" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Game_Executable</t>
+  </si>
+  <si>
+    <t>mike</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100B6C98-D2EA-4787-B524-363DAFEAEF43}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +465,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Null coelesce and excel changes
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CEF00F-67E5-46AB-81DD-329BF32AE176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7589C2D-5096-40DC-921F-CF6FDFA43D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1245" windowWidth="24240" windowHeight="13140" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -426,7 +426,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,9 +487,6 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Setting up convention for multiple threads based on gamers
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7589C2D-5096-40DC-921F-CF6FDFA43D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7709FBF3-2A9F-4AF0-8531-C3A7DE0F96C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1245" windowWidth="24240" windowHeight="13140" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
+    <workbookView xWindow="28410" yWindow="2415" windowWidth="24300" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>mike</t>
+  </si>
+  <si>
+    <t>eddie</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100B6C98-D2EA-4787-B524-363DAFEAEF43}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +491,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
refactoring, organizing and interpreting data, pushing data to excel sheets
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7709FBF3-2A9F-4AF0-8531-C3A7DE0F96C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E958955-C480-449F-8D46-D6A45E3690E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28410" yWindow="2415" windowWidth="24300" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
+    <workbookView xWindow="1335" yWindow="3090" windowWidth="24300" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Mac_Address</t>
   </si>
@@ -53,9 +50,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>Processes</t>
-  </si>
-  <si>
     <t>ComputerName</t>
   </si>
   <si>
@@ -66,6 +60,18 @@
   </si>
   <si>
     <t>eddie</t>
+  </si>
+  <si>
+    <t>Processes(separate by comma)</t>
+  </si>
+  <si>
+    <t>cheatengine.exe</t>
+  </si>
+  <si>
+    <t>mikesunique.exe</t>
+  </si>
+  <si>
+    <t>Name(Must Be unique)</t>
   </si>
 </sst>
 </file>
@@ -429,11 +435,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -444,73 +451,79 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactoring, setting pulse convention for process retrieval, and adding bad process cache load
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E958955-C480-449F-8D46-D6A45E3690E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF9DFFD-4054-45D6-A33E-8C41049F0517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="3090" windowWidth="24300" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
+    <workbookView xWindow="990" yWindow="2745" windowWidth="24300" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Mac_Address</t>
   </si>
@@ -72,13 +72,43 @@
   </si>
   <si>
     <t>Name(Must Be unique)</t>
+  </si>
+  <si>
+    <t>LAPTOP-GB79J0R7</t>
+  </si>
+  <si>
+    <t>192.168.1.25</t>
+  </si>
+  <si>
+    <t>dummyEd</t>
+  </si>
+  <si>
+    <t>DESKTOP-LB66A9H</t>
+  </si>
+  <si>
+    <t>192.168.1.3</t>
+  </si>
+  <si>
+    <t>mmcquad.17@gmail.com</t>
+  </si>
+  <si>
+    <t>dummyMike</t>
+  </si>
+  <si>
+    <t>DESKTOP-STQI345</t>
+  </si>
+  <si>
+    <t>192.168.1.20</t>
+  </si>
+  <si>
+    <t>dummymikeunique.exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +120,25 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,14 +161,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100B6C98-D2EA-4787-B524-363DAFEAEF43}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,8 +497,8 @@
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
   </cols>
@@ -480,19 +534,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>8008</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -505,20 +559,20 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -527,8 +581,38 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{3E36D2A1-F277-44D3-97B5-9BA5749CE3C9}"/>
+    <hyperlink ref="E4" r:id="rId2" display="mmcquad.17@gmail.com" xr:uid="{97F6E79F-C023-4AFA-88B1-476E2F5D4D2A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code cleanup and Front end feedback with updates on gamer status
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF9DFFD-4054-45D6-A33E-8C41049F0517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A89C39F-0734-470D-8B2B-A4DE20F2D218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="2745" windowWidth="24300" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
+    <workbookView xWindow="28680" yWindow="1245" windowWidth="24240" windowHeight="13140" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Mac_Address</t>
   </si>
@@ -489,7 +489,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,10 +595,10 @@
         <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>1717</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -610,7 +610,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{3E36D2A1-F277-44D3-97B5-9BA5749CE3C9}"/>
-    <hyperlink ref="E4" r:id="rId2" display="mmcquad.17@gmail.com" xr:uid="{97F6E79F-C023-4AFA-88B1-476E2F5D4D2A}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{7FEAEE20-1382-4604-A9B1-D7BD38788BAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>

<commit_message>
code cleanup, asynch watch, directories and files, button flow,
</commit_message>
<xml_diff>
--- a/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
+++ b/Seniordesign/bin/Debug/ExcelFiles/SeniorDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmcqu\Source\repos\Seniordesign\Seniordesign\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A89C39F-0734-470D-8B2B-A4DE20F2D218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDDFFF6-A42F-4A58-A3AC-A1D56979E9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1245" windowWidth="24240" windowHeight="13140" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21885" windowHeight="11385" xr2:uid="{D475F130-1F67-44C0-A0F3-8F90E6609115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
-  <si>
-    <t>Mac_Address</t>
-  </si>
-  <si>
-    <t>IP_Address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Password</t>
   </si>
@@ -62,15 +56,9 @@
     <t>eddie</t>
   </si>
   <si>
-    <t>Processes(separate by comma)</t>
-  </si>
-  <si>
     <t>cheatengine.exe</t>
   </si>
   <si>
-    <t>mikesunique.exe</t>
-  </si>
-  <si>
     <t>Name(Must Be unique)</t>
   </si>
   <si>
@@ -80,9 +68,6 @@
     <t>192.168.1.25</t>
   </si>
   <si>
-    <t>dummyEd</t>
-  </si>
-  <si>
     <t>DESKTOP-LB66A9H</t>
   </si>
   <si>
@@ -102,6 +87,18 @@
   </si>
   <si>
     <t>dummymikeunique.exe</t>
+  </si>
+  <si>
+    <t>Ed Greenlee</t>
+  </si>
+  <si>
+    <t>Inserted_Processes(seperate by comma)</t>
+  </si>
+  <si>
+    <t>IP_Address(optional)</t>
+  </si>
+  <si>
+    <t>mikesunique.exe,miketwo.exe</t>
   </si>
 </sst>
 </file>
@@ -486,131 +483,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100B6C98-D2EA-4787-B524-363DAFEAEF43}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>8008</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>2447</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>8008</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>1717</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{3E36D2A1-F277-44D3-97B5-9BA5749CE3C9}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{7FEAEE20-1382-4604-A9B1-D7BD38788BAA}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BC4D0101-2D77-45B6-9D2B-D2AEFAA5E7AB}"/>
+    <hyperlink ref="D4" r:id="rId2" display="mmcquad.17@gmail.com" xr:uid="{DC40E3DE-AB82-4A6C-8C99-654C479CC199}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>